<commit_message>
Add arch_regions data for low arch
</commit_message>
<xml_diff>
--- a/message_ix_buildings/data/chilled/version/dle_coolssp/arch_regions.xlsx
+++ b/message_ix_buildings/data/chilled/version/dle_coolssp/arch_regions.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iiasahub.sharepoint.com/sites/ene/dle/Shared Documents/WS2 - Documents/Analysis/Climate impacts and space conditioning/Data/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meas/iiasagit/message-ix-buildings/message_ix_buildings/data/chilled/version/dle_coolssp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="8_{0BC07357-14C0-499C-8410-CA5621DFA114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D86BF75-F58D-4C2A-9EC4-6FC45F63077F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F9EC61-1B38-EE40-AEC9-27E39240A093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="2" r:id="rId1"/>
     <sheet name="exist" sheetId="1" r:id="rId2"/>
+    <sheet name="low" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="19">
   <si>
     <t>REGION_GEA</t>
   </si>
@@ -85,6 +86,9 @@
   </si>
   <si>
     <t>new</t>
+  </si>
+  <si>
+    <t>low</t>
   </si>
 </sst>
 </file>
@@ -927,15 +931,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E93E0A-AFFA-4A67-A7AB-B0E26E753F9B}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.76953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.40625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -952,7 +956,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -969,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -988,7 +992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1007,7 +1011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1026,7 +1030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1045,7 +1049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1064,7 +1068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1083,7 +1087,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1102,7 +1106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1121,7 +1125,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1140,7 +1144,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1169,15 +1173,15 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="5" width="10.40625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1211,7 +1215,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1230,7 +1234,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1249,7 +1253,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1268,7 +1272,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1287,7 +1291,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1306,7 +1310,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1325,7 +1329,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1344,7 +1348,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1363,7 +1367,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1382,7 +1386,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1399,6 +1403,255 @@
       <c r="E12">
         <f t="shared" si="0"/>
         <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA98C439-67D8-6D4F-9996-B41963DE85DD}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>44</v>
+      </c>
+      <c r="E2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="str">
+        <f>C2</f>
+        <v>low</v>
+      </c>
+      <c r="D3">
+        <f>D2+2</f>
+        <v>46</v>
+      </c>
+      <c r="E3">
+        <f>E2+2</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C12" si="0">C3</f>
+        <v>low</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:E12" si="1">D3+2</f>
+        <v>48</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>low</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>low</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>low</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>low</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>low</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>low</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>low</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>low</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1407,26 +1660,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="46547ee6-6ca2-4afd-a080-da8f16d2cd0c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7055cb63-5b6a-447a-8f70-ef29d578b7b7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D19E63A46B5DA3429C25EA571CE0F796" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e679349038a4754d11970580dd46bd2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7055cb63-5b6a-447a-8f70-ef29d578b7b7" xmlns:ns3="71aff983-82d3-474b-a127-0471d4604477" xmlns:ns4="46547ee6-6ca2-4afd-a080-da8f16d2cd0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="650f812ef2478dc891b5ff7b5dc3f19d" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="7055cb63-5b6a-447a-8f70-ef29d578b7b7"/>
@@ -1680,10 +1913,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="46547ee6-6ca2-4afd-a080-da8f16d2cd0c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7055cb63-5b6a-447a-8f70-ef29d578b7b7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8238EC7F-9B9F-462B-81CC-89566FB03354}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{307D1318-A1F6-4D71-AAEA-D7C6A108F7DD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7055cb63-5b6a-447a-8f70-ef29d578b7b7"/>
+    <ds:schemaRef ds:uri="71aff983-82d3-474b-a127-0471d4604477"/>
+    <ds:schemaRef ds:uri="46547ee6-6ca2-4afd-a080-da8f16d2cd0c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1701,10 +1966,15 @@
     <ds:schemaRef ds:uri="71aff983-82d3-474b-a127-0471d4604477"/>
     <ds:schemaRef ds:uri="7055cb63-5b6a-447a-8f70-ef29d578b7b7"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="46547ee6-6ca2-4afd-a080-da8f16d2cd0c"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{307D1318-A1F6-4D71-AAEA-D7C6A108F7DD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8238EC7F-9B9F-462B-81CC-89566FB03354}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>